<commit_message>
fix(pipelining): fix testing programs #18
</commit_message>
<xml_diff>
--- a/programs/pipelining/pipeliningregandramhazards.xlsx
+++ b/programs/pipelining/pipeliningregandramhazards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\pipelining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4929D726-AD32-4B54-A8F2-E0D375FDEC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4992F9E8-82A9-4C55-A498-59FE2E234D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{283EBD8D-59D5-476D-AFCF-7CC67732E96E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{283EBD8D-59D5-476D-AFCF-7CC67732E96E}"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t>Immediate</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>ST</t>
+  </si>
+  <si>
+    <t>MOV R0, #0 ROR 0</t>
   </si>
 </sst>
 </file>
@@ -527,7 +530,7 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="A8:B11"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,7 +787,7 @@
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -817,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="3">
         <v>0</v>
@@ -832,11 +835,11 @@
         <v>0</v>
       </c>
       <c r="R8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8" s="3" t="str">
         <f>DEC2HEX(C8*2^15 + D8*2^14 + E8*2^13 + F8*2^12 + G8*2^11 + H8*2^10 + I8*2^9 + J8*2^8 + K8*2^7 + L8*2^6 + M8*2^5 + N8*2^4 + O8 * 2 ^ 3 + P8  * 2^2 + Q8 * 2 + R8)</f>
-        <v>8221</v>
+        <v>8200</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
@@ -871,7 +874,7 @@
         <v>1</v>
       </c>
       <c r="K9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" s="3">
         <v>1</v>
@@ -886,17 +889,17 @@
         <v>0</v>
       </c>
       <c r="P9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q9" s="3">
         <v>0</v>
       </c>
       <c r="R9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S9" s="3" t="str">
         <f t="shared" ref="S9:S10" si="0">DEC2HEX(C9*2^15 + D9*2^14 + E9*2^13 + F9*2^12 + G9*2^11 + H9*2^10 + I9*2^9 + J9*2^8 + K9*2^7 + L9*2^6 + M9*2^5 + N9*2^4 + O9 * 2 ^ 3 + P9  * 2^2 + Q9 * 2 + R9)</f>
-        <v>BC1</v>
+        <v>B44</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
@@ -1043,6 +1046,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="I5:R5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:P6"/>
+    <mergeCell ref="Q6:R6"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="K2:M2"/>
@@ -1052,16 +1065,6 @@
     <mergeCell ref="K3:N3"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="M4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="I5:R5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1069,10 +1072,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51EAB318-5794-4230-B6C4-3E439CA2E766}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1080,7 +1083,7 @@
     <col min="2" max="2" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1097,7 +1100,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1117,7 +1120,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1137,23 +1140,23 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>38</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>35</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>36</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>